<commit_message>
didnt save excel spreadsheet before last commit.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WordTemplate\Word-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6D3E4-0822-4E1B-93F5-0213E9BD612B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A529F-5121-4B26-9A5D-9E4133A3181F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{982A6973-8D7D-4542-94F3-53A8385ECBE1}"/>
   </bookViews>
@@ -244,61 +244,61 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.4142135623730951</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7320508075688772</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2360679774997898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4494897427831779</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6457513110645907</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8284271247461903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1622776601683795</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3166247903553998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4641016151377544</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6055512754639891</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7416573867739413</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.872983346207417</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>256</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>289</c:v>
+                  <c:v>4.1231056256176606</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>324</c:v>
+                  <c:v>4.2426406871192848</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>361</c:v>
+                  <c:v>4.358898943540674</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400</c:v>
+                  <c:v>4.4721359549995796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>A2^2</f>
+        <f>A2^(1/2)</f>
         <v>0</v>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0">A3^2</f>
+        <f t="shared" ref="B3:B22" si="0">A3^(1/2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1.7320508075688772</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>2.2360679774997898</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>2.4494897427831779</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>2.6457513110645907</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>2.8284271247461903</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>3.1622776601683795</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>3.3166247903553998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>3.4641016151377544</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>169</v>
+        <v>3.6055512754639891</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>3.7416573867739413</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>3.872983346207417</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>289</v>
+        <v>4.1231056256176606</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>4.2426406871192848</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>361</v>
+        <v>4.358898943540674</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>4.4721359549995796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>